<commit_message>
Added reporting section Credentials in config file
</commit_message>
<xml_diff>
--- a/src/main/java/com/pwc/qa/testdata/PwCTestData.xlsx
+++ b/src/main/java/com/pwc/qa/testdata/PwCTestData.xlsx
@@ -1,51 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19380" windowHeight="6420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19380" windowHeight="6420" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="2" r:id="rId1"/>
     <sheet name="login" sheetId="3" r:id="rId2"/>
+    <sheet name="business" sheetId="4" r:id="rId3"/>
+    <sheet name="sub" sheetId="5" r:id="rId4"/>
+    <sheet name="datalist" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:M10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
-  <si>
-    <t>Companyname</t>
-  </si>
-  <si>
-    <t>Companypan</t>
-  </si>
-  <si>
-    <t>ZBCLL4390X</t>
-  </si>
-  <si>
-    <t>URCLL4390V</t>
-  </si>
-  <si>
-    <t>XNCLL4390J</t>
-  </si>
-  <si>
-    <t>IPCLL4390U</t>
-  </si>
-  <si>
-    <t>Wipro</t>
-  </si>
-  <si>
-    <t>PWCUltra</t>
-  </si>
-  <si>
-    <t>Electrotherm</t>
-  </si>
-  <si>
-    <t>Voltas</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>test123</t>
   </si>
@@ -70,12 +44,69 @@
   <si>
     <t>A@SS1234</t>
   </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Business Unit Name</t>
+  </si>
+  <si>
+    <t>Sub Business Unit Name</t>
+  </si>
+  <si>
+    <t>company1</t>
+  </si>
+  <si>
+    <t>Unit01</t>
+  </si>
+  <si>
+    <t>sub01</t>
+  </si>
+  <si>
+    <t>Business Unit</t>
+  </si>
+  <si>
+    <t>unit01</t>
+  </si>
+  <si>
+    <t>Company PAN</t>
+  </si>
+  <si>
+    <t>CMNPK4241N</t>
+  </si>
+  <si>
+    <t>KMNPK8241P</t>
+  </si>
+  <si>
+    <t>company2</t>
+  </si>
+  <si>
+    <t>KMNPK9241R</t>
+  </si>
+  <si>
+    <t>company3</t>
+  </si>
+  <si>
+    <t>KRPPK9241N</t>
+  </si>
+  <si>
+    <t>company4</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,7 +244,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -248,7 +278,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,57 +453,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -483,73 +512,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2">
         <v>1234566</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -563,4 +590,109 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>